<commit_message>
Description: COMANDO PARA VERFICAR TIKET MÉDIO
</commit_message>
<xml_diff>
--- a/DashBoard/Projeto+1+-+Dashboard+de+vendas.xlsx
+++ b/DashBoard/Projeto+1+-+Dashboard+de+vendas.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\HD\ESTUDOS EM GERAL GRADE 1 SEMENTRES 2025\SQL PARA ANALISTA DE DADOS\Projeto DashBoard de acompanhamento de vendas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\HD\ESTUDOS EM GERAL GRADE 1 SEMENTRES 2025\SQL PARA ANALISTA DE DADOS\Projeto DashBoard de acompanhamento de vendas\Project\DashBoard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4D8D7BC-9C7D-470B-BD7A-39B8CFF32DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C576969-6F83-409F-892C-26753CCDEF30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,14 +19,12 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Resultados!$M$3:$N$3</definedName>
-    <definedName name="_xlchart.v5.0" hidden="1">Resultados!$I$3:$J$3</definedName>
-    <definedName name="_xlchart.v5.1" hidden="1">Resultados!$I$4:$J$8</definedName>
-    <definedName name="_xlchart.v5.2" hidden="1">Resultados!$K$3</definedName>
-    <definedName name="_xlchart.v5.3" hidden="1">Resultados!$K$4:$K$8</definedName>
-    <definedName name="_xlchart.v5.4" hidden="1">Dashboard!$O$12</definedName>
-    <definedName name="_xlchart.v5.5" hidden="1">Dashboard!$O$13</definedName>
-    <definedName name="_xlchart.v5.6" hidden="1">Dashboard!$O$12</definedName>
-    <definedName name="_xlchart.v5.7" hidden="1">Dashboard!$O$13</definedName>
+    <definedName name="_xlchart.v5.0" hidden="1">Dashboard!$O$12</definedName>
+    <definedName name="_xlchart.v5.1" hidden="1">Dashboard!$O$13</definedName>
+    <definedName name="_xlchart.v5.2" hidden="1">Resultados!$I$3:$J$3</definedName>
+    <definedName name="_xlchart.v5.3" hidden="1">Resultados!$I$4:$J$8</definedName>
+    <definedName name="_xlchart.v5.4" hidden="1">Resultados!$K$3</definedName>
+    <definedName name="_xlchart.v5.5" hidden="1">Resultados!$K$4:$K$8</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>mês</t>
   </si>
@@ -59,9 +57,6 @@
   </si>
   <si>
     <t>receita (k, R$)</t>
-  </si>
-  <si>
-    <t>conversão (%)</t>
   </si>
   <si>
     <t>ticket médio (k, R$)</t>
@@ -102,14 +97,21 @@
   <si>
     <t>5 - Dias da semana com maior número de visitas ao site</t>
   </si>
+  <si>
+    <t>Vendas (#)</t>
+  </si>
+  <si>
+    <t>Conversão (%)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
     <numFmt numFmtId="165" formatCode="[$-416]mmm\-yy;@"/>
+    <numFmt numFmtId="175" formatCode="0.0"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -168,16 +170,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="17" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -186,6 +184,27 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="175" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -387,6 +406,42 @@
               <c:numCache>
                 <c:formatCode>[$-416]mmm\-yy;@</c:formatCode>
                 <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>44075</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44105</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44136</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44166</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44197</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44228</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44256</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44287</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44317</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44348</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44378</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44409</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -396,6 +451,42 @@
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>931</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1207</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1008</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1058</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1932</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2376</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3819</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4440</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6130</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6353</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -429,7 +520,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>conversão (%)</c:v>
+                  <c:v>Conversão (%)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -515,6 +606,42 @@
               <c:numCache>
                 <c:formatCode>[$-416]mmm\-yy;@</c:formatCode>
                 <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>44075</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44105</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44136</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44166</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44197</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44228</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44256</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44287</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44317</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44348</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44378</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44409</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -524,6 +651,42 @@
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.19230769230769201</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.7593984962405999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.6454018227009097E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.2738095238095198E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.0245746691871401E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.2307692307692298E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.15942028985507E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.97643097643097E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.103168368682901</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.132657657657657</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.17504078303425699</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.19738706123091401</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -547,7 +710,7 @@
         <c:axId val="1886420143"/>
         <c:axId val="1886418895"/>
       </c:lineChart>
-      <c:catAx>
+      <c:dateAx>
         <c:axId val="1305806031"/>
         <c:scaling>
           <c:orientation val="minMax"/>
@@ -594,10 +757,9 @@
         <c:crossAx val="1305802703"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="1"/>
-      </c:catAx>
+        <c:baseTimeUnit val="months"/>
+      </c:dateAx>
       <c:valAx>
         <c:axId val="1305802703"/>
         <c:scaling>
@@ -696,7 +858,7 @@
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
-      <c:catAx>
+      <c:dateAx>
         <c:axId val="1886420143"/>
         <c:scaling>
           <c:orientation val="minMax"/>
@@ -710,10 +872,9 @@
         <c:crossAx val="1886418895"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="1"/>
-      </c:catAx>
+        <c:baseTimeUnit val="months"/>
+      </c:dateAx>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -972,6 +1133,42 @@
               <c:numCache>
                 <c:formatCode>[$-416]mmm\-yy;@</c:formatCode>
                 <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>44075</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44105</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44136</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44166</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44197</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44228</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44256</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44287</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44317</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44348</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44378</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44409</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -979,8 +1176,44 @@
             <c:numRef>
               <c:f>Resultados!$E$4:$E$15</c:f>
               <c:numCache>
-                <c:formatCode>#,##0</c:formatCode>
+                <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>259.29000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1676.45685</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2278.5075000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2602.7686899999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2297.2240499999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3631.0958999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7911.1924799999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7477.5559199999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>21508.476480000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>33179.246639999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>58987.786489999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>68274.090230000002</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1100,6 +1333,42 @@
               <c:numCache>
                 <c:formatCode>[$-416]mmm\-yy;@</c:formatCode>
                 <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>44075</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44105</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44136</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44166</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44197</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44228</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44256</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44287</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44317</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44348</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44378</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44409</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1107,8 +1376,44 @@
             <c:numRef>
               <c:f>Resultados!$G$4:$G$15</c:f>
               <c:numCache>
-                <c:formatCode>#,##0.0</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>51.857999999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>47.898767142857103</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>51.784261363636297</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>78.871778484848406</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>71.788251562499994</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>53.398469117646997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>66.480609075630198</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>52.658844507042197</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>54.590041827411099</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>56.331488353140898</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>54.974637921714802</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>54.445048030302999</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1132,7 +1437,7 @@
         <c:axId val="1886420143"/>
         <c:axId val="1886418895"/>
       </c:lineChart>
-      <c:catAx>
+      <c:dateAx>
         <c:axId val="1305806031"/>
         <c:scaling>
           <c:orientation val="minMax"/>
@@ -1179,10 +1484,9 @@
         <c:crossAx val="1305802703"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="1"/>
-      </c:catAx>
+        <c:baseTimeUnit val="months"/>
+      </c:dateAx>
       <c:valAx>
         <c:axId val="1305802703"/>
         <c:scaling>
@@ -1204,7 +1508,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1246,7 +1550,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="r"/>
-        <c:numFmt formatCode="#,##0.0" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1281,7 +1585,7 @@
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
-      <c:catAx>
+      <c:dateAx>
         <c:axId val="1886420143"/>
         <c:scaling>
           <c:orientation val="minMax"/>
@@ -1295,10 +1599,9 @@
         <c:crossAx val="1886418895"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="1"/>
-      </c:catAx>
+        <c:baseTimeUnit val="months"/>
+      </c:dateAx>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -2331,12 +2634,12 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v5.1</cx:f>
-        <cx:nf>_xlchart.v5.0</cx:nf>
+        <cx:f>_xlchart.v5.3</cx:f>
+        <cx:nf>_xlchart.v5.2</cx:nf>
       </cx:strDim>
       <cx:numDim type="colorVal">
-        <cx:f>_xlchart.v5.3</cx:f>
-        <cx:nf>_xlchart.v5.2</cx:nf>
+        <cx:f>_xlchart.v5.5</cx:f>
+        <cx:nf>_xlchart.v5.4</cx:nf>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -2374,7 +2677,7 @@
         <cx:series layoutId="regionMap" uniqueId="{02A53EDD-DCFC-4A88-B213-71274D6215FF}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v5.2</cx:f>
+              <cx:f>_xlchart.v5.4</cx:f>
               <cx:v>vendas (#)</cx:v>
             </cx:txData>
           </cx:tx>
@@ -2409,8 +2712,8 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="colorVal">
-        <cx:f>_xlchart.v5.7</cx:f>
-        <cx:nf>_xlchart.v5.6</cx:nf>
+        <cx:f>_xlchart.v5.1</cx:f>
+        <cx:nf>_xlchart.v5.0</cx:nf>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -6535,8 +6838,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="12579803" y="206829"/>
-              <a:ext cx="4572000" cy="4991100"/>
+              <a:off x="12558032" y="206829"/>
+              <a:ext cx="4561114" cy="4991100"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -7337,11 +7640,11 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.28515625" customWidth="1"/>
-    <col min="2" max="2" width="21" style="9" customWidth="1"/>
+    <col min="2" max="2" width="21" style="5" customWidth="1"/>
     <col min="3" max="4" width="21" customWidth="1"/>
-    <col min="5" max="5" width="21" style="7" customWidth="1"/>
-    <col min="6" max="6" width="21" style="3" customWidth="1"/>
-    <col min="7" max="7" width="21" style="5" customWidth="1"/>
+    <col min="5" max="5" width="21" style="4" customWidth="1"/>
+    <col min="6" max="6" width="21" style="2" customWidth="1"/>
+    <col min="7" max="7" width="21" style="3" customWidth="1"/>
     <col min="9" max="9" width="14.28515625" customWidth="1"/>
     <col min="10" max="11" width="15.85546875" customWidth="1"/>
     <col min="13" max="13" width="20" customWidth="1"/>
@@ -7367,13 +7670,17 @@
   <dimension ref="B2:U30"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="7" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+    <col min="5" max="5" width="35.28515625" customWidth="1"/>
+    <col min="6" max="6" width="34" customWidth="1"/>
+    <col min="7" max="7" width="35.85546875" customWidth="1"/>
     <col min="8" max="8" width="7.7109375" customWidth="1"/>
     <col min="9" max="11" width="10.7109375" customWidth="1"/>
     <col min="12" max="12" width="7.7109375" customWidth="1"/>
@@ -7384,79 +7691,91 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="M2" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="M2" s="12" t="s">
+      <c r="P2" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="P2" s="12" t="s">
+      <c r="S2" s="8" t="s">
         <v>16</v>
-      </c>
-      <c r="S2" s="12" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="3" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="6" t="s">
+      <c r="D3" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="I3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="N3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="Q3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="S3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="T3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="T3" s="1" t="s">
+      <c r="U3" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="U3" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="4" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B4" s="8"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="4"/>
+      <c r="B4" s="9">
+        <v>44075</v>
+      </c>
+      <c r="C4" s="11">
+        <v>26</v>
+      </c>
+      <c r="D4" s="11">
+        <v>5</v>
+      </c>
+      <c r="E4" s="15">
+        <v>259.29000000000002</v>
+      </c>
+      <c r="F4" s="12">
+        <v>0.19230769230769201</v>
+      </c>
+      <c r="G4" s="14">
+        <v>51.857999999999997</v>
+      </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
@@ -7469,12 +7788,24 @@
       <c r="U4" s="1"/>
     </row>
     <row r="5" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B5" s="8"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="4"/>
+      <c r="B5" s="9">
+        <v>44105</v>
+      </c>
+      <c r="C5" s="11">
+        <v>931</v>
+      </c>
+      <c r="D5" s="11">
+        <v>35</v>
+      </c>
+      <c r="E5" s="15">
+        <v>1676.45685</v>
+      </c>
+      <c r="F5" s="12">
+        <v>3.7593984962405999E-2</v>
+      </c>
+      <c r="G5" s="14">
+        <v>47.898767142857103</v>
+      </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
@@ -7487,12 +7818,24 @@
       <c r="U5" s="1"/>
     </row>
     <row r="6" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B6" s="8"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="4"/>
+      <c r="B6" s="9">
+        <v>44136</v>
+      </c>
+      <c r="C6" s="11">
+        <v>1207</v>
+      </c>
+      <c r="D6" s="11">
+        <v>44</v>
+      </c>
+      <c r="E6" s="15">
+        <v>2278.5075000000002</v>
+      </c>
+      <c r="F6" s="12">
+        <v>3.6454018227009097E-2</v>
+      </c>
+      <c r="G6" s="14">
+        <v>51.784261363636297</v>
+      </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
@@ -7505,12 +7848,24 @@
       <c r="U6" s="1"/>
     </row>
     <row r="7" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B7" s="8"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="4"/>
+      <c r="B7" s="9">
+        <v>44166</v>
+      </c>
+      <c r="C7" s="11">
+        <v>1008</v>
+      </c>
+      <c r="D7" s="11">
+        <v>33</v>
+      </c>
+      <c r="E7" s="15">
+        <v>2602.7686899999999</v>
+      </c>
+      <c r="F7" s="12">
+        <v>3.2738095238095198E-2</v>
+      </c>
+      <c r="G7" s="14">
+        <v>78.871778484848406</v>
+      </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
@@ -7523,12 +7878,24 @@
       <c r="U7" s="1"/>
     </row>
     <row r="8" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B8" s="8"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="4"/>
+      <c r="B8" s="9">
+        <v>44197</v>
+      </c>
+      <c r="C8" s="11">
+        <v>1058</v>
+      </c>
+      <c r="D8" s="11">
+        <v>32</v>
+      </c>
+      <c r="E8" s="15">
+        <v>2297.2240499999998</v>
+      </c>
+      <c r="F8" s="12">
+        <v>3.0245746691871401E-2</v>
+      </c>
+      <c r="G8" s="14">
+        <v>71.788251562499994</v>
+      </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
@@ -7541,129 +7908,213 @@
       <c r="U8" s="1"/>
     </row>
     <row r="9" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B9" s="8"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="4"/>
+      <c r="B9" s="9">
+        <v>44228</v>
+      </c>
+      <c r="C9" s="11">
+        <v>1300</v>
+      </c>
+      <c r="D9" s="11">
+        <v>68</v>
+      </c>
+      <c r="E9" s="15">
+        <v>3631.0958999999998</v>
+      </c>
+      <c r="F9" s="12">
+        <v>5.2307692307692298E-2</v>
+      </c>
+      <c r="G9" s="14">
+        <v>53.398469117646997</v>
+      </c>
       <c r="S9" s="1"/>
       <c r="T9" s="1"/>
       <c r="U9" s="1"/>
     </row>
     <row r="10" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B10" s="8"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="4"/>
+      <c r="B10" s="9">
+        <v>44256</v>
+      </c>
+      <c r="C10" s="11">
+        <v>1932</v>
+      </c>
+      <c r="D10" s="11">
+        <v>119</v>
+      </c>
+      <c r="E10" s="15">
+        <v>7911.1924799999997</v>
+      </c>
+      <c r="F10" s="12">
+        <v>6.15942028985507E-2</v>
+      </c>
+      <c r="G10" s="14">
+        <v>66.480609075630198</v>
+      </c>
       <c r="S10" s="1"/>
       <c r="T10" s="1"/>
       <c r="U10" s="1"/>
     </row>
     <row r="11" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B11" s="8"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="4"/>
+      <c r="B11" s="9">
+        <v>44287</v>
+      </c>
+      <c r="C11" s="11">
+        <v>2376</v>
+      </c>
+      <c r="D11" s="11">
+        <v>142</v>
+      </c>
+      <c r="E11" s="15">
+        <v>7477.5559199999998</v>
+      </c>
+      <c r="F11" s="12">
+        <v>5.97643097643097E-2</v>
+      </c>
+      <c r="G11" s="14">
+        <v>52.658844507042197</v>
+      </c>
     </row>
     <row r="12" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B12" s="8"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="4"/>
+      <c r="B12" s="9">
+        <v>44317</v>
+      </c>
+      <c r="C12" s="11">
+        <v>3819</v>
+      </c>
+      <c r="D12" s="11">
+        <v>394</v>
+      </c>
+      <c r="E12" s="15">
+        <v>21508.476480000001</v>
+      </c>
+      <c r="F12" s="12">
+        <v>0.103168368682901</v>
+      </c>
+      <c r="G12" s="14">
+        <v>54.590041827411099</v>
+      </c>
     </row>
     <row r="13" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B13" s="8"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="4"/>
+      <c r="B13" s="9">
+        <v>44348</v>
+      </c>
+      <c r="C13" s="11">
+        <v>4440</v>
+      </c>
+      <c r="D13" s="11">
+        <v>589</v>
+      </c>
+      <c r="E13" s="15">
+        <v>33179.246639999998</v>
+      </c>
+      <c r="F13" s="12">
+        <v>0.132657657657657</v>
+      </c>
+      <c r="G13" s="14">
+        <v>56.331488353140898</v>
+      </c>
     </row>
     <row r="14" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B14" s="8"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="4"/>
+      <c r="B14" s="9">
+        <v>44378</v>
+      </c>
+      <c r="C14" s="11">
+        <v>6130</v>
+      </c>
+      <c r="D14" s="11">
+        <v>1073</v>
+      </c>
+      <c r="E14" s="15">
+        <v>58987.786489999999</v>
+      </c>
+      <c r="F14" s="12">
+        <v>0.17504078303425699</v>
+      </c>
+      <c r="G14" s="14">
+        <v>54.974637921714802</v>
+      </c>
     </row>
     <row r="15" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B15" s="8"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="4"/>
+      <c r="B15" s="9">
+        <v>44409</v>
+      </c>
+      <c r="C15" s="11">
+        <v>6353</v>
+      </c>
+      <c r="D15" s="11">
+        <v>1254</v>
+      </c>
+      <c r="E15" s="15">
+        <v>68274.090230000002</v>
+      </c>
+      <c r="F15" s="12">
+        <v>0.19738706123091401</v>
+      </c>
+      <c r="G15" s="14">
+        <v>54.445048030302999</v>
+      </c>
     </row>
     <row r="29" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C29" s="10">
+      <c r="C29" s="6">
         <v>44075</v>
       </c>
-      <c r="D29" s="10">
+      <c r="D29" s="6">
         <f>EDATE(C29,1)</f>
         <v>44105</v>
       </c>
-      <c r="E29" s="10">
+      <c r="E29" s="6">
         <f t="shared" ref="E29:L29" si="0">EDATE(D29,1)</f>
         <v>44136</v>
       </c>
-      <c r="F29" s="10">
+      <c r="F29" s="6">
         <f t="shared" si="0"/>
         <v>44166</v>
       </c>
-      <c r="G29" s="10">
+      <c r="G29" s="6">
         <f t="shared" si="0"/>
         <v>44197</v>
       </c>
-      <c r="H29" s="10">
+      <c r="H29" s="6">
         <f t="shared" si="0"/>
         <v>44228</v>
       </c>
-      <c r="I29" s="10">
+      <c r="I29" s="6">
         <f t="shared" si="0"/>
         <v>44256</v>
       </c>
-      <c r="J29" s="10">
+      <c r="J29" s="6">
         <f t="shared" si="0"/>
         <v>44287</v>
       </c>
-      <c r="K29" s="10">
+      <c r="K29" s="6">
         <f t="shared" si="0"/>
         <v>44317</v>
       </c>
-      <c r="L29" s="10">
+      <c r="L29" s="6">
         <f t="shared" si="0"/>
         <v>44348</v>
       </c>
-      <c r="M29" s="10">
+      <c r="M29" s="6">
         <f t="shared" ref="M29:N29" si="1">EDATE(L29,1)</f>
         <v>44378</v>
       </c>
-      <c r="N29" s="10">
+      <c r="N29" s="6">
         <f t="shared" si="1"/>
         <v>44409</v>
       </c>
     </row>
     <row r="30" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="11"/>
-      <c r="I30" s="11"/>
-      <c r="J30" s="11"/>
-      <c r="K30" s="11"/>
-      <c r="L30" s="11"/>
-      <c r="M30" s="11"/>
-      <c r="N30" s="11"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="7"/>
+      <c r="J30" s="7"/>
+      <c r="K30" s="7"/>
+      <c r="L30" s="7"/>
+      <c r="M30" s="7"/>
+      <c r="N30" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>